<commit_message>
switch between hedge types
</commit_message>
<xml_diff>
--- a/Logik Base-Peak Produkte inkl Cal-Q.xlsx
+++ b/Logik Base-Peak Produkte inkl Cal-Q.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bkwfmbenergie-my.sharepoint.com/personal/daniel_aeberhard_bkw_ch/Documents/Desktop/EnergyUtils/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{EE7FC5F0-D7C6-4F95-80B7-B89A03A802E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B869A177-C519-4489-B39E-7EF0AABA0F8D}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{EE7FC5F0-D7C6-4F95-80B7-B89A03A802E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F4F4466-A9A7-4D2D-B318-89C276D9E484}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="780" windowWidth="27750" windowHeight="19230" activeTab="1" xr2:uid="{CF2CAE9D-B578-4E60-B720-896D1366AE3F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{CF2CAE9D-B578-4E60-B720-896D1366AE3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Base-Peak" sheetId="1" r:id="rId1"/>
@@ -2603,8 +2603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58B22230-2F22-44B8-B5B2-63687FC12290}">
   <dimension ref="D3:V27"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="U5" sqref="U5:U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3250,7 +3250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9F739C5-A558-412C-8192-3FA1FCA3BE95}">
   <dimension ref="B3:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" activeCellId="1" sqref="D10:D11 D5:D6"/>
     </sheetView>
   </sheetViews>

</xml_diff>